<commit_message>
chore: Generate package lock file and update auxiliary spreadsheet.
</commit_message>
<xml_diff>
--- a/CONTROLES POR COMISSÃO E GESTORES.xlsx
+++ b/CONTROLES POR COMISSÃO E GESTORES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDIÇÕES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Desktop\SEIOP - DER\DEMANDAS AVULSAS\CÉSAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6C9A79-28A2-49C4-9EDD-A69FA2027760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9090BD-F863-4517-8BDF-249F87825FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="454" xr2:uid="{B96EB9A8-6169-46F2-89FD-740783B0C7B5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="454" xr2:uid="{B96EB9A8-6169-46F2-89FD-740783B0C7B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,20 +611,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -703,7 +689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -834,15 +820,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -868,23 +845,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -914,12 +880,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -927,19 +889,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -948,71 +901,65 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1022,658 +969,6 @@
   <dxfs count="78">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1696,7 +991,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1705,6 +1000,714 @@
         </right>
         <top/>
         <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3178,21 +3181,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E49DCA8C-BF3E-4A50-9685-635EA2C8AC88}" name="Tabela3" displayName="Tabela3" ref="B34:K50" totalsRowCount="1" headerRowDxfId="25" dataDxfId="23" totalsRowDxfId="21" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E49DCA8C-BF3E-4A50-9685-635EA2C8AC88}" name="Tabela3" displayName="Tabela3" ref="B34:K50" totalsRowCount="1" headerRowDxfId="0" dataDxfId="24" totalsRowDxfId="22" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="21">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B35:F49">
     <sortCondition ref="B34:B49"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7C167C76-67AF-4A26-8B9A-BCE2A4995E2A}" name="GESTOR(A)_x000a_ATUANTE" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{884CD221-7FDF-449F-BDDC-36A59A961922}" name="GESTOR SUPLENTE" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{4BAEAB60-D8F3-4A1C-A2A7-1AF80D70ECFB}" name="FISCAL NOMEADO" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{92B91F80-B146-424A-9B8F-B3A204D6D240}" name="MUNICIPIO" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{536E627B-103D-43E3-ADF4-5534C1B8AC84}" name="EMPRESA" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{6244ECFF-D04A-4C9E-9BB6-3E00642A9BA0}" name="%EXEC" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{E519A9AE-567A-406C-B69A-B1B53C257A70}" name="STATUS" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{682B89AE-0AB9-4B7F-8C3B-66D341320532}" name="FISCAL SUPLENTE" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{B76C21C5-382B-4784-B00B-25BF832EBF82}" name="ADM" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{E184221B-D39C-481A-9EF0-7BBC0BDCFFB3}" name="ADM SUPLENTE" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7C167C76-67AF-4A26-8B9A-BCE2A4995E2A}" name="GESTOR(A)_x000a_ATUANTE" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{884CD221-7FDF-449F-BDDC-36A59A961922}" name="GESTOR SUPLENTE" dataDxfId="9" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{4BAEAB60-D8F3-4A1C-A2A7-1AF80D70ECFB}" name="FISCAL NOMEADO" dataDxfId="8" totalsRowDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{92B91F80-B146-424A-9B8F-B3A204D6D240}" name="MUNICIPIO" dataDxfId="7" totalsRowDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{536E627B-103D-43E3-ADF4-5534C1B8AC84}" name="EMPRESA" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{6244ECFF-D04A-4C9E-9BB6-3E00642A9BA0}" name="%EXEC" dataDxfId="5" totalsRowDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{E519A9AE-567A-406C-B69A-B1B53C257A70}" name="STATUS" dataDxfId="4" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{682B89AE-0AB9-4B7F-8C3B-66D341320532}" name="FISCAL SUPLENTE" dataDxfId="3" totalsRowDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{B76C21C5-382B-4784-B00B-25BF832EBF82}" name="ADM" dataDxfId="2" totalsRowDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{E184221B-D39C-481A-9EF0-7BBC0BDCFFB3}" name="ADM SUPLENTE" dataDxfId="1" totalsRowDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3519,7 +3522,7 @@
   <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3536,30 +3539,30 @@
     <col min="10" max="11" width="19.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="1.5703125" style="4" customWidth="1"/>
     <col min="13" max="13" width="37.85546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="3" style="42" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" style="30" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="34.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="44"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="32"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3595,7 +3598,7 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="44" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -3604,7 +3607,7 @@
       <c r="C3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -3613,7 +3616,7 @@
       <c r="F3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="27">
         <v>0.25580000000000003</v>
       </c>
       <c r="H3" s="6" t="s">
@@ -3630,7 +3633,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="45" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3639,7 +3642,7 @@
       <c r="C4" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -3648,7 +3651,7 @@
       <c r="F4" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="27">
         <v>0</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -3665,7 +3668,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="44" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3674,7 +3677,7 @@
       <c r="C5" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -3683,7 +3686,7 @@
       <c r="F5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="27">
         <v>0.99670000000000003</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -3700,7 +3703,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="45" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3709,7 +3712,7 @@
       <c r="C6" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -3718,7 +3721,7 @@
       <c r="F6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="27">
         <v>0.97860000000000003</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -3734,10 +3737,10 @@
         <v>135</v>
       </c>
       <c r="M6"/>
-      <c r="N6" s="43"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -3746,7 +3749,7 @@
       <c r="C7" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -3755,7 +3758,7 @@
       <c r="F7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="27">
         <v>1.6500000000000001E-2</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -3771,10 +3774,10 @@
         <v>135</v>
       </c>
       <c r="M7"/>
-      <c r="N7" s="43"/>
+      <c r="N7" s="31"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -3783,7 +3786,7 @@
       <c r="C8" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -3792,7 +3795,7 @@
       <c r="F8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="27">
         <v>0.38669999999999999</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -3808,10 +3811,10 @@
         <v>135</v>
       </c>
       <c r="M8"/>
-      <c r="N8" s="43"/>
+      <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="44" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -3820,7 +3823,7 @@
       <c r="C9" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="24" t="s">
         <v>152</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -3829,7 +3832,7 @@
       <c r="F9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="27">
         <v>0.9899</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -3846,7 +3849,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="45" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -3855,7 +3858,7 @@
       <c r="C10" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -3864,7 +3867,7 @@
       <c r="F10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="27">
         <v>3.7699999999999997E-2</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -3881,7 +3884,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="44" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -3890,7 +3893,7 @@
       <c r="C11" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -3899,7 +3902,7 @@
       <c r="F11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="27">
         <v>0.88560000000000005</v>
       </c>
       <c r="H11" s="6" t="s">
@@ -3916,7 +3919,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3925,7 +3928,7 @@
       <c r="C12" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -3934,7 +3937,7 @@
       <c r="F12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="27">
         <v>0.53190000000000004</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -3951,7 +3954,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="44" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -3960,7 +3963,7 @@
       <c r="C13" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="24" t="s">
         <v>146</v>
       </c>
       <c r="E13" s="6" t="s">
@@ -3969,7 +3972,7 @@
       <c r="F13" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="27">
         <v>0.1074</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -3986,7 +3989,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="45" t="s">
         <v>110</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -3995,7 +3998,7 @@
       <c r="C14" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E14" s="6" t="s">
@@ -4004,7 +4007,7 @@
       <c r="F14" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="27">
         <v>0.54500000000000004</v>
       </c>
       <c r="H14" s="6" t="s">
@@ -4021,7 +4024,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="44" t="s">
         <v>96</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4030,7 +4033,7 @@
       <c r="C15" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -4039,7 +4042,7 @@
       <c r="F15" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="27">
         <v>0.64100000000000001</v>
       </c>
       <c r="H15" s="6" t="s">
@@ -4056,7 +4059,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="45" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -4065,7 +4068,7 @@
       <c r="C16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="24" t="s">
         <v>147</v>
       </c>
       <c r="E16" s="6" t="s">
@@ -4074,7 +4077,7 @@
       <c r="F16" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="27">
         <v>0.71809999999999996</v>
       </c>
       <c r="H16" s="6" t="s">
@@ -4091,7 +4094,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="44" t="s">
         <v>98</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4100,7 +4103,7 @@
       <c r="C17" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="24" t="s">
         <v>147</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -4109,7 +4112,7 @@
       <c r="F17" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="27">
         <v>0.62</v>
       </c>
       <c r="H17" s="6" t="s">
@@ -4126,7 +4129,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="45" t="s">
         <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -4135,7 +4138,7 @@
       <c r="C18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="24" t="s">
         <v>147</v>
       </c>
       <c r="E18" s="6" t="s">
@@ -4144,7 +4147,7 @@
       <c r="F18" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="27">
         <v>0.2321</v>
       </c>
       <c r="H18" s="6" t="s">
@@ -4161,7 +4164,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -4170,7 +4173,7 @@
       <c r="C19" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="24" t="s">
         <v>150</v>
       </c>
       <c r="E19" s="6" t="s">
@@ -4179,7 +4182,7 @@
       <c r="F19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="27">
         <v>1</v>
       </c>
       <c r="H19" s="6" t="s">
@@ -4196,7 +4199,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="45" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -4205,7 +4208,7 @@
       <c r="C20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="24" t="s">
         <v>147</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -4214,7 +4217,7 @@
       <c r="F20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="27">
         <v>0</v>
       </c>
       <c r="H20" s="6" t="s">
@@ -4231,7 +4234,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="44" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -4240,7 +4243,7 @@
       <c r="C21" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="24" t="s">
         <v>150</v>
       </c>
       <c r="E21" s="6" t="s">
@@ -4249,7 +4252,7 @@
       <c r="F21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="27">
         <v>0.78049999999999997</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -4266,7 +4269,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="45" t="s">
         <v>121</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -4275,7 +4278,7 @@
       <c r="C22" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="24" t="s">
         <v>147</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -4284,7 +4287,7 @@
       <c r="F22" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="26">
         <v>0.5</v>
       </c>
       <c r="H22" s="6" t="s">
@@ -4301,7 +4304,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="44" t="s">
         <v>118</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -4310,7 +4313,7 @@
       <c r="C23" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E23" s="6" t="s">
@@ -4319,7 +4322,7 @@
       <c r="F23" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="27">
         <v>1</v>
       </c>
       <c r="H23" s="6" t="s">
@@ -4336,7 +4339,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -4345,7 +4348,7 @@
       <c r="C24" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="24" t="s">
         <v>150</v>
       </c>
       <c r="E24" s="6" t="s">
@@ -4354,7 +4357,7 @@
       <c r="F24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="27">
         <v>0.7903</v>
       </c>
       <c r="H24" s="6" t="s">
@@ -4371,7 +4374,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="44" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -4380,7 +4383,7 @@
       <c r="C25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="24" t="s">
         <v>149</v>
       </c>
       <c r="E25" s="6" t="s">
@@ -4389,7 +4392,7 @@
       <c r="F25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="27">
         <v>0.78090000000000004</v>
       </c>
       <c r="H25" s="6" t="s">
@@ -4406,7 +4409,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="45" t="s">
         <v>111</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -4415,7 +4418,7 @@
       <c r="C26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="24" t="s">
         <v>150</v>
       </c>
       <c r="E26" s="6" t="s">
@@ -4424,7 +4427,7 @@
       <c r="F26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="27">
         <v>0.66039999999999999</v>
       </c>
       <c r="H26" s="6" t="s">
@@ -4441,7 +4444,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="44" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -4450,7 +4453,7 @@
       <c r="C27" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="24" t="s">
         <v>150</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -4459,7 +4462,7 @@
       <c r="F27" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="27">
         <v>0.86519999999999997</v>
       </c>
       <c r="H27" s="6" t="s">
@@ -4476,7 +4479,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="45" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -4485,7 +4488,7 @@
       <c r="C28" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="24" t="s">
         <v>150</v>
       </c>
       <c r="E28" s="6" t="s">
@@ -4494,7 +4497,7 @@
       <c r="F28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="27">
         <v>0.69730000000000003</v>
       </c>
       <c r="H28" s="6" t="s">
@@ -4527,8 +4530,8 @@
       <c r="J29" s="9"/>
       <c r="K29" s="11"/>
       <c r="M29"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
     </row>
     <row r="30" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
@@ -4563,7 +4566,7 @@
       <c r="M31"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="21"/>
+      <c r="C32" s="19"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
@@ -4572,60 +4575,60 @@
       <c r="M32"/>
     </row>
     <row r="33" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="45"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="33"/>
       <c r="M33"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K34" s="18" t="s">
         <v>134</v>
       </c>
       <c r="L34"/>
     </row>
     <row r="35" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="44" t="s">
         <v>112</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -4643,24 +4646,24 @@
       <c r="F35" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="33">
+      <c r="G35" s="27">
         <v>1</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H35" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I35" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="K35" s="18" t="s">
+      <c r="K35" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="45" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -4678,13 +4681,13 @@
       <c r="F36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="33">
+      <c r="G36" s="27">
         <v>0.5746</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I36" s="18" t="s">
+      <c r="I36" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J36" s="6" t="s">
@@ -4695,7 +4698,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="44" t="s">
         <v>75</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -4713,13 +4716,13 @@
       <c r="F37" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G37" s="33">
+      <c r="G37" s="27">
         <v>0.84570000000000001</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="H37" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I37" s="18" t="s">
+      <c r="I37" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J37" s="6" t="s">
@@ -4730,7 +4733,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="45" t="s">
         <v>76</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -4748,13 +4751,13 @@
       <c r="F38" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G38" s="33">
+      <c r="G38" s="27">
         <v>0.99929999999999997</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I38" s="18" t="s">
+      <c r="I38" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J38" s="6" t="s">
@@ -4765,7 +4768,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="44" t="s">
         <v>77</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -4783,13 +4786,13 @@
       <c r="F39" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G39" s="33">
+      <c r="G39" s="27">
         <v>0.79930000000000001</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H39" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I39" s="18" t="s">
+      <c r="I39" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J39" s="6" t="s">
@@ -4800,7 +4803,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="45" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -4818,13 +4821,13 @@
       <c r="F40" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G40" s="33">
+      <c r="G40" s="27">
         <v>0.30669999999999997</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I40" s="18" t="s">
+      <c r="I40" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J40" s="6" t="s">
@@ -4835,7 +4838,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="44" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -4853,13 +4856,13 @@
       <c r="F41" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G41" s="33">
+      <c r="G41" s="27">
         <v>0.96009999999999995</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="H41" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I41" s="18" t="s">
+      <c r="I41" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J41" s="6" t="s">
@@ -4870,7 +4873,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="45" t="s">
         <v>115</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -4888,13 +4891,13 @@
       <c r="F42" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G42" s="33">
+      <c r="G42" s="27">
         <v>1.5408999999999999</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I42" s="18" t="s">
+      <c r="I42" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J42" s="6" t="s">
@@ -4905,7 +4908,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="44" t="s">
         <v>80</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -4923,13 +4926,13 @@
       <c r="F43" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G43" s="33">
+      <c r="G43" s="27">
         <v>0.78459999999999996</v>
       </c>
-      <c r="H43" s="18" t="s">
+      <c r="H43" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I43" s="18" t="s">
+      <c r="I43" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J43" s="6" t="s">
@@ -4940,7 +4943,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="45" t="s">
         <v>113</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -4958,13 +4961,13 @@
       <c r="F44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G44" s="33">
+      <c r="G44" s="27">
         <v>1</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="I44" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J44" s="6" t="s">
@@ -4975,7 +4978,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="44" t="s">
         <v>81</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -4993,13 +4996,13 @@
       <c r="F45" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G45" s="33">
+      <c r="G45" s="27">
         <v>0.89959999999999996</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H45" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I45" s="18" t="s">
+      <c r="I45" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J45" s="6" t="s">
@@ -5008,13 +5011,13 @@
       <c r="K45" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="M45" s="53" t="s">
+      <c r="M45" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="N45" s="53"/>
+      <c r="N45" s="40"/>
     </row>
     <row r="46" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="45" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -5032,13 +5035,13 @@
       <c r="F46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="33">
+      <c r="G46" s="27">
         <v>0.97130000000000005</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="I46" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J46" s="6" t="s">
@@ -5047,10 +5050,10 @@
       <c r="K46" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="M46" s="23" t="s">
+      <c r="M46" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="N46" s="46">
+      <c r="N46" s="34">
         <f>COUNTIF(Tabela1[GESTOR(A)
 ATUANTE],M46)+COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],M46)+COUNTIF(Tabela3[GESTOR(A)
@@ -5059,7 +5062,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="44" t="s">
         <v>130</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5077,13 +5080,13 @@
       <c r="F47" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="G47" s="33">
+      <c r="G47" s="27">
         <v>0.80789999999999995</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I47" s="18" t="s">
+      <c r="I47" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J47" s="6" t="s">
@@ -5092,10 +5095,10 @@
       <c r="K47" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="M47" s="23" t="s">
+      <c r="M47" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="N47" s="46">
+      <c r="N47" s="34">
         <f>COUNTIF(Tabela1[GESTOR(A)
 ATUANTE],M47)+COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],M47)+COUNTIF(Tabela3[GESTOR(A)
@@ -5104,7 +5107,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="45" t="s">
         <v>83</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -5122,13 +5125,13 @@
       <c r="F48" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G48" s="33">
+      <c r="G48" s="27">
         <v>0.60799999999999998</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I48" s="18" t="s">
+      <c r="I48" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J48" s="6" t="s">
@@ -5137,10 +5140,10 @@
       <c r="K48" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="M48" s="23" t="s">
+      <c r="M48" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="N48" s="46">
+      <c r="N48" s="34">
         <f>COUNTIF(Tabela1[GESTOR(A)
 ATUANTE],M48)+COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],M48)+COUNTIF(Tabela3[GESTOR(A)
@@ -5149,7 +5152,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="44" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -5161,31 +5164,31 @@
       <c r="D49" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G49" s="34">
+      <c r="G49" s="27">
         <v>0.14130000000000001</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="H49" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="I49" s="18" t="s">
+      <c r="I49" s="6" t="s">
         <v>145</v>
       </c>
       <c r="J49" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="K49" s="9" t="s">
+      <c r="K49" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="M49" s="23" t="s">
+      <c r="M49" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="N49" s="46">
+      <c r="N49" s="34">
         <f>COUNTIF(Tabela1[GESTOR(A)
 ATUANTE],M49)+COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],M49)+COUNTIF(Tabela3[GESTOR(A)
@@ -5194,10 +5197,10 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="30"/>
+      <c r="C50" s="25"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="10">
@@ -5209,10 +5212,10 @@
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
-      <c r="M50" s="23" t="s">
+      <c r="M50" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="N50" s="46">
+      <c r="N50" s="34">
         <f>COUNTIF(Tabela1[GESTOR(A)
 ATUANTE],M50)+COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],M50)+COUNTIF(Tabela3[GESTOR(A)
@@ -5230,7 +5233,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="4"/>
-      <c r="M51" s="42"/>
+      <c r="M51" s="30"/>
     </row>
     <row r="52" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
@@ -5242,36 +5245,36 @@
         <v>14</v>
       </c>
       <c r="G52" s="4"/>
-      <c r="M52" s="42"/>
+      <c r="M52" s="30"/>
     </row>
     <row r="53" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="D53" s="21"/>
+      <c r="D53" s="19"/>
       <c r="G53" s="4"/>
-      <c r="M53" s="42"/>
+      <c r="M53" s="30"/>
     </row>
     <row r="54" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="55"/>
-      <c r="H54" s="55"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="55"/>
-      <c r="K54" s="56"/>
-      <c r="L54" s="44"/>
-      <c r="M54" s="52" t="s">
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="42"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="32"/>
+      <c r="M54" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="N54" s="52"/>
-      <c r="O54" s="47"/>
+      <c r="N54" s="39"/>
+      <c r="O54" s="35"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -5286,7 +5289,7 @@
       <c r="E55" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F55" s="20" t="s">
+      <c r="F55" s="18" t="s">
         <v>24</v>
       </c>
       <c r="G55" s="2" t="s">
@@ -5295,48 +5298,48 @@
       <c r="H55" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="I55" s="20" t="s">
+      <c r="I55" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J55" s="20" t="s">
+      <c r="J55" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="K55" s="20" t="s">
+      <c r="K55" s="18" t="s">
         <v>134</v>
       </c>
       <c r="L55"/>
-      <c r="M55" s="48" t="s">
+      <c r="M55" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="N55" s="50" cm="1">
+      <c r="N55" s="37" cm="1">
         <f t="array" ref="N55">SUMPRODUCT(IF(ISERROR(FIND(M55, $D$3:$D$69)), 0, 1))</f>
         <v>12</v>
       </c>
-      <c r="O55" s="43"/>
+      <c r="O55" s="31"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="20" t="s">
         <v>142</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E56" s="23" t="s">
+      <c r="E56" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="F56" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G56" s="35">
+      <c r="G56" s="28">
         <v>0.6603</v>
       </c>
-      <c r="H56" s="30" t="s">
+      <c r="H56" s="25" t="s">
         <v>163</v>
       </c>
       <c r="I56" s="6" t="s">
@@ -5349,38 +5352,38 @@
         <v>144</v>
       </c>
       <c r="L56"/>
-      <c r="M56" s="48" t="s">
+      <c r="M56" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="N56" s="50" cm="1">
+      <c r="N56" s="37" cm="1">
         <f t="array" ref="N56">SUMPRODUCT(IF(ISERROR(FIND(M56, $D$3:$D$69)), 0, 1))</f>
         <v>19</v>
       </c>
-      <c r="O56" s="43"/>
+      <c r="O56" s="31"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="20" t="s">
         <v>142</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="D57" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E57" s="23" t="s">
+      <c r="E57" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F57" s="23" t="s">
+      <c r="F57" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="G57" s="35">
+      <c r="G57" s="28">
         <v>0.51629999999999998</v>
       </c>
-      <c r="H57" s="23" t="s">
+      <c r="H57" s="21" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="6" t="s">
@@ -5393,38 +5396,38 @@
         <v>135</v>
       </c>
       <c r="L57"/>
-      <c r="M57" s="48" t="s">
+      <c r="M57" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="N57" s="50" cm="1">
+      <c r="N57" s="37" cm="1">
         <f t="array" ref="N57">SUMPRODUCT(IF(ISERROR(FIND(M57, $D$3:$D$69)), 0, 1))</f>
         <v>5</v>
       </c>
-      <c r="O57" s="43"/>
+      <c r="O57" s="31"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="20" t="s">
         <v>142</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D58" s="23" t="s">
+      <c r="D58" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="E58" s="23" t="s">
+      <c r="E58" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="F58" s="23" t="s">
+      <c r="F58" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="G58" s="35">
+      <c r="G58" s="28">
         <v>0.99219999999999997</v>
       </c>
-      <c r="H58" s="23" t="s">
+      <c r="H58" s="21" t="s">
         <v>164</v>
       </c>
       <c r="I58" s="6" t="s">
@@ -5437,38 +5440,38 @@
         <v>135</v>
       </c>
       <c r="L58"/>
-      <c r="M58" s="48" t="s">
+      <c r="M58" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="N58" s="50" cm="1">
+      <c r="N58" s="37" cm="1">
         <f t="array" ref="N58">SUMPRODUCT(IF(ISERROR(FIND(M58, $D$3:$D$69)), 0, 1))</f>
         <v>6</v>
       </c>
-      <c r="O58" s="43"/>
+      <c r="O58" s="31"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="20" t="s">
         <v>142</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="23" t="s">
+      <c r="D59" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E59" s="23" t="s">
+      <c r="E59" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F59" s="23" t="s">
+      <c r="F59" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="G59" s="35">
+      <c r="G59" s="28">
         <v>0.99539999999999995</v>
       </c>
-      <c r="H59" s="23" t="s">
+      <c r="H59" s="21" t="s">
         <v>164</v>
       </c>
       <c r="I59" s="6" t="s">
@@ -5481,38 +5484,38 @@
         <v>135</v>
       </c>
       <c r="L59"/>
-      <c r="M59" s="48" t="s">
+      <c r="M59" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="N59" s="50" cm="1">
+      <c r="N59" s="37" cm="1">
         <f t="array" ref="N59">SUMPRODUCT(IF(ISERROR(FIND(M59, $D$3:$D$69)), 0, 1))</f>
         <v>15</v>
       </c>
-      <c r="O59" s="43"/>
+      <c r="O59" s="31"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="20" t="s">
         <v>142</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="23" t="s">
+      <c r="D60" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E60" s="23" t="s">
+      <c r="E60" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F60" s="23" t="s">
+      <c r="F60" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="G60" s="35">
+      <c r="G60" s="28">
         <v>0.43519999999999998</v>
       </c>
-      <c r="H60" s="23" t="s">
+      <c r="H60" s="21" t="s">
         <v>163</v>
       </c>
       <c r="I60" s="6" t="s">
@@ -5525,17 +5528,17 @@
         <v>135</v>
       </c>
       <c r="L60"/>
-      <c r="M60" s="48" t="s">
+      <c r="M60" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="N60" s="50" cm="1">
+      <c r="N60" s="37" cm="1">
         <f t="array" ref="N60">SUMPRODUCT(IF(ISERROR(FIND(M60, $D$3:$D$69)), 0, 1))</f>
         <v>18</v>
       </c>
-      <c r="O60" s="43"/>
+      <c r="O60" s="31"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="27" t="s">
+      <c r="A61" s="47" t="s">
         <v>52</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -5544,19 +5547,19 @@
       <c r="C61" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="23" t="s">
+      <c r="D61" s="21" t="s">
         <v>158</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F61" s="23" t="s">
+      <c r="F61" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G61" s="35">
+      <c r="G61" s="28">
         <v>0.5958</v>
       </c>
-      <c r="H61" s="23" t="s">
+      <c r="H61" s="21" t="s">
         <v>163</v>
       </c>
       <c r="I61" s="6" t="s">
@@ -5569,17 +5572,17 @@
         <v>135</v>
       </c>
       <c r="L61"/>
-      <c r="M61" s="23" t="s">
+      <c r="M61" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="N61" s="50" cm="1">
+      <c r="N61" s="37" cm="1">
         <f t="array" ref="N61">SUMPRODUCT(IF(ISERROR(FIND(M61, $D$3:$D$69)), 0, 1))</f>
         <v>21</v>
       </c>
-      <c r="O61" s="43"/>
+      <c r="O61" s="31"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="46" t="s">
         <v>53</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -5588,19 +5591,19 @@
       <c r="C62" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="23" t="s">
+      <c r="D62" s="21" t="s">
         <v>158</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F62" s="23" t="s">
+      <c r="F62" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G62" s="35">
+      <c r="G62" s="28">
         <v>0.84209999999999996</v>
       </c>
-      <c r="H62" s="23" t="s">
+      <c r="H62" s="21" t="s">
         <v>163</v>
       </c>
       <c r="I62" s="6" t="s">
@@ -5613,143 +5616,143 @@
         <v>135</v>
       </c>
       <c r="L62"/>
-      <c r="M62" s="23" t="s">
+      <c r="M62" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="N62" s="50" cm="1">
+      <c r="N62" s="37" cm="1">
         <f t="array" ref="N62">SUMPRODUCT(IF(ISERROR(FIND(M62, $D$3:$D$69)), 0, 1))</f>
         <v>1</v>
       </c>
-      <c r="O62" s="43"/>
+      <c r="O62" s="31"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="F63" s="24" t="s">
+      <c r="F63" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="G63" s="36">
+      <c r="G63" s="29">
         <v>0</v>
       </c>
-      <c r="H63" s="24" t="s">
+      <c r="H63" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="I63" s="16" t="s">
+      <c r="I63" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="J63" s="16" t="str">
+      <c r="J63" s="15" t="str">
         <f t="shared" ref="J63:J69" si="0">UPPER("REJANE VASCONCELOS")</f>
         <v>REJANE VASCONCELOS</v>
       </c>
-      <c r="K63" s="16" t="s">
+      <c r="K63" s="15" t="s">
         <v>135</v>
       </c>
       <c r="L63"/>
-      <c r="M63" s="23" t="s">
+      <c r="M63" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="N63" s="50" cm="1">
+      <c r="N63" s="37" cm="1">
         <f t="array" ref="N63">SUMPRODUCT(IF(ISERROR(FIND(M63, $D$3:$D$69)), 0, 1))</f>
         <v>13</v>
       </c>
-      <c r="O63" s="43"/>
+      <c r="O63" s="31"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E64" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F64" s="24" t="s">
+      <c r="F64" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G64" s="36">
+      <c r="G64" s="29">
         <v>0.85919999999999996</v>
       </c>
-      <c r="H64" s="24" t="s">
+      <c r="H64" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="I64" s="16" t="s">
+      <c r="I64" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="J64" s="16" t="str">
+      <c r="J64" s="15" t="str">
         <f t="shared" si="0"/>
         <v>REJANE VASCONCELOS</v>
       </c>
-      <c r="K64" s="16" t="s">
+      <c r="K64" s="15" t="s">
         <v>135</v>
       </c>
       <c r="L64"/>
-      <c r="M64" s="43"/>
-      <c r="N64" s="43"/>
-      <c r="O64" s="43"/>
+      <c r="M64" s="31"/>
+      <c r="N64" s="31"/>
+      <c r="O64" s="31"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="E65" s="16" t="str">
+      <c r="E65" s="15" t="str">
         <f>UPPER("Miguel Pereira")</f>
         <v>MIGUEL PEREIRA</v>
       </c>
-      <c r="F65" s="24" t="s">
+      <c r="F65" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="36">
+      <c r="G65" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H65" s="24" t="s">
+      <c r="H65" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="I65" s="16" t="s">
+      <c r="I65" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="J65" s="16" t="str">
+      <c r="J65" s="15" t="str">
         <f t="shared" si="0"/>
         <v>REJANE VASCONCELOS</v>
       </c>
-      <c r="K65" s="16" t="s">
+      <c r="K65" s="15" t="s">
         <v>135</v>
       </c>
       <c r="L65"/>
-      <c r="M65" s="42"/>
-      <c r="N65" s="43"/>
-      <c r="O65" s="43"/>
+      <c r="M65" s="30"/>
+      <c r="N65" s="31"/>
+      <c r="O65" s="31"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="40" t="s">
+      <c r="A66" s="46" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -5764,16 +5767,16 @@
       <c r="E66" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F66" s="23" t="s">
+      <c r="F66" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="G66" s="35">
+      <c r="G66" s="28">
         <v>0.87860000000000005</v>
       </c>
-      <c r="H66" s="23" t="s">
+      <c r="H66" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I66" s="23" t="s">
+      <c r="I66" s="21" t="s">
         <v>157</v>
       </c>
       <c r="J66" s="6" t="str">
@@ -5784,11 +5787,11 @@
         <v>135</v>
       </c>
       <c r="M66"/>
-      <c r="N66" s="43"/>
-      <c r="O66" s="43"/>
+      <c r="N66" s="31"/>
+      <c r="O66" s="31"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="27" t="s">
+      <c r="A67" s="47" t="s">
         <v>123</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -5803,16 +5806,16 @@
       <c r="E67" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F67" s="23" t="s">
+      <c r="F67" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="G67" s="35">
+      <c r="G67" s="28">
         <v>0</v>
       </c>
-      <c r="H67" s="23" t="s">
+      <c r="H67" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I67" s="23" t="s">
+      <c r="I67" s="21" t="s">
         <v>157</v>
       </c>
       <c r="J67" s="6" t="str">
@@ -5825,7 +5828,7 @@
       <c r="M67"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="40" t="s">
+      <c r="A68" s="46" t="s">
         <v>55</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -5840,16 +5843,16 @@
       <c r="E68" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F68" s="23" t="s">
+      <c r="F68" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="35">
+      <c r="G68" s="28">
         <v>0.97019999999999995</v>
       </c>
-      <c r="H68" s="23" t="s">
+      <c r="H68" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I68" s="23" t="s">
+      <c r="I68" s="21" t="s">
         <v>157</v>
       </c>
       <c r="J68" s="6" t="str">
@@ -5862,7 +5865,7 @@
       <c r="M68"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="27" t="s">
+      <c r="A69" s="47" t="s">
         <v>56</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -5877,16 +5880,16 @@
       <c r="E69" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F69" s="23" t="s">
+      <c r="F69" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="G69" s="35">
+      <c r="G69" s="28">
         <v>0.31530000000000002</v>
       </c>
-      <c r="H69" s="23" t="s">
+      <c r="H69" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I69" s="23" t="s">
+      <c r="I69" s="21" t="s">
         <v>157</v>
       </c>
       <c r="J69" s="6" t="str">
@@ -5899,7 +5902,7 @@
       <c r="M69"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="8" t="s">
         <v>71</v>
       </c>
@@ -5926,7 +5929,7 @@
 ATUANTE],B71)</f>
         <v>7</v>
       </c>
-      <c r="N71" s="43"/>
+      <c r="N71" s="31"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
@@ -5937,10 +5940,10 @@
 ATUANTE],B72)</f>
         <v>7</v>
       </c>
-      <c r="N72" s="43"/>
+      <c r="N72" s="31"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N73" s="43"/>
+      <c r="N73" s="31"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B74"/>
@@ -5948,68 +5951,68 @@
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74"/>
-      <c r="N74" s="43"/>
+      <c r="N74" s="31"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D75" s="25"/>
+      <c r="D75" s="23"/>
       <c r="E75"/>
       <c r="F75"/>
-      <c r="N75" s="43"/>
+      <c r="N75" s="31"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E76"/>
       <c r="F76"/>
-      <c r="N76" s="43"/>
+      <c r="N76" s="31"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E77"/>
       <c r="F77"/>
-      <c r="N77" s="43"/>
+      <c r="N77" s="31"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E78"/>
       <c r="F78"/>
-      <c r="N78" s="43"/>
+      <c r="N78" s="31"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E79"/>
       <c r="F79"/>
-      <c r="N79" s="43"/>
+      <c r="N79" s="31"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G80" s="4"/>
-      <c r="N80" s="43"/>
+      <c r="N80" s="31"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
       <c r="G81" s="4"/>
-      <c r="N81" s="43"/>
+      <c r="N81" s="31"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="G82" s="4"/>
-      <c r="N82" s="43"/>
+      <c r="N82" s="31"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G83" s="4"/>
-      <c r="N83" s="43"/>
+      <c r="N83" s="31"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G84" s="4"/>
-      <c r="N84" s="43"/>
+      <c r="N84" s="31"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G85" s="4"/>
-      <c r="N85" s="43"/>
+      <c r="N85" s="31"/>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E86"/>
       <c r="F86"/>
-      <c r="N86" s="43"/>
+      <c r="N86" s="31"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H90"/>
@@ -6054,7 +6057,7 @@
     <mergeCell ref="M45:N45"/>
     <mergeCell ref="A54:K54"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.15748031496062992" bottom="0.15748031496062992" header="0.15748031496062992" footer="0.15748031496062992"/>
   <pageSetup paperSize="8" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
chore: update works report for managers and inspectors
</commit_message>
<xml_diff>
--- a/CONTROLES POR COMISSÃO E GESTORES.xlsx
+++ b/CONTROLES POR COMISSÃO E GESTORES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Desktop\SEIOP - DER\DEMANDAS AVULSAS\CÉSAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDICOES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9090BD-F863-4517-8BDF-249F87825FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0340A459-02F2-4CB2-8DAF-A2D293433B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="454" xr2:uid="{B96EB9A8-6169-46F2-89FD-740783B0C7B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="454" xr2:uid="{B96EB9A8-6169-46F2-89FD-740783B0C7B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="171">
   <si>
     <t>GESTOR(A)
 ATUANTE</t>
@@ -542,9 +542,6 @@
   </si>
   <si>
     <t>ANDREIA VASQUES / ISADORA ROSALINO</t>
-  </si>
-  <si>
-    <t>ANDREIA VASQUES / LUCIANA POSTIÇO</t>
   </si>
   <si>
     <t>%EXEC</t>
@@ -925,6 +922,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -943,30 +958,1007 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="78">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1087,7 +2079,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1100,12 +2092,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1120,7 +2106,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1139,850 +2125,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2021,42 +2163,40 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2078,17 +2218,12 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2103,119 +2238,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2248,34 +2273,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3163,16 +3160,16 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77490B51-49AC-48CE-B9D3-F5913D37C0FB}" name="Tabela2" displayName="Tabela2" ref="B55:K70" totalsRowCount="1" headerRowDxfId="51" dataDxfId="49" totalsRowDxfId="47" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="46">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{C168971F-8A1F-4CE0-AB1A-A91564F865A1}" name="GESTOR(A)_x000a_ATUANTE" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{28D500DA-BD33-447D-801C-1EDBD59B514A}" name="GESTOR SUPLENTE" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{1BC929D7-C79E-4DD8-8692-AEFFFF4E2201}" name="FISCAL NOMEADO" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{6DB822D5-3B20-4BEB-9FA9-33D9AE724FF4}" name="MUNICIPIO" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{1DE280A2-C1B5-497D-B2A7-425CC71F3653}" name="EMPRESA" totalsRowFunction="count" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{95ED015E-6AEE-4CBF-A570-2665B6975A98}" name="%EXEC" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{1C47120A-915F-4E95-BA45-AF0C41018F09}" name="STATUS" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{0C9C4230-87B4-46C7-8DFF-3C0A2F340B11}" name="FISCAL SUPLENTE" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{4E783EA6-0DCE-4695-BBAF-E24638D55153}" name="ADM" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{CE385090-95B6-4F49-A43B-E7EB63C58B59}" name="ADM SUPLENTE" dataDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="1" xr3:uid="{C168971F-8A1F-4CE0-AB1A-A91564F865A1}" name="GESTOR(A)_x000a_ATUANTE" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{28D500DA-BD33-447D-801C-1EDBD59B514A}" name="GESTOR SUPLENTE" dataDxfId="44" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1BC929D7-C79E-4DD8-8692-AEFFFF4E2201}" name="FISCAL NOMEADO" dataDxfId="43" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{6DB822D5-3B20-4BEB-9FA9-33D9AE724FF4}" name="MUNICIPIO" dataDxfId="42" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{1DE280A2-C1B5-497D-B2A7-425CC71F3653}" name="EMPRESA" totalsRowFunction="count" dataDxfId="41" totalsRowDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{95ED015E-6AEE-4CBF-A570-2665B6975A98}" name="%EXEC" dataDxfId="40" totalsRowDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{1C47120A-915F-4E95-BA45-AF0C41018F09}" name="STATUS" dataDxfId="39" totalsRowDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{0C9C4230-87B4-46C7-8DFF-3C0A2F340B11}" name="FISCAL SUPLENTE" dataDxfId="38" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{4E783EA6-0DCE-4695-BBAF-E24638D55153}" name="ADM" dataDxfId="37" totalsRowDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{CE385090-95B6-4F49-A43B-E7EB63C58B59}" name="ADM SUPLENTE" dataDxfId="36" totalsRowDxfId="0">
       <calculatedColumnFormula>UPPER("Rejane Vasconcelos Cristino")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3181,21 +3178,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E49DCA8C-BF3E-4A50-9685-635EA2C8AC88}" name="Tabela3" displayName="Tabela3" ref="B34:K50" totalsRowCount="1" headerRowDxfId="0" dataDxfId="24" totalsRowDxfId="22" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E49DCA8C-BF3E-4A50-9685-635EA2C8AC88}" name="Tabela3" displayName="Tabela3" ref="B34:K50" totalsRowCount="1" headerRowDxfId="35" dataDxfId="33" totalsRowDxfId="31" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="30">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B35:F49">
     <sortCondition ref="B34:B49"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{7C167C76-67AF-4A26-8B9A-BCE2A4995E2A}" name="GESTOR(A)_x000a_ATUANTE" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{884CD221-7FDF-449F-BDDC-36A59A961922}" name="GESTOR SUPLENTE" dataDxfId="9" totalsRowDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{4BAEAB60-D8F3-4A1C-A2A7-1AF80D70ECFB}" name="FISCAL NOMEADO" dataDxfId="8" totalsRowDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{92B91F80-B146-424A-9B8F-B3A204D6D240}" name="MUNICIPIO" dataDxfId="7" totalsRowDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{536E627B-103D-43E3-ADF4-5534C1B8AC84}" name="EMPRESA" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{6244ECFF-D04A-4C9E-9BB6-3E00642A9BA0}" name="%EXEC" dataDxfId="5" totalsRowDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{E519A9AE-567A-406C-B69A-B1B53C257A70}" name="STATUS" dataDxfId="4" totalsRowDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{682B89AE-0AB9-4B7F-8C3B-66D341320532}" name="FISCAL SUPLENTE" dataDxfId="3" totalsRowDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{B76C21C5-382B-4784-B00B-25BF832EBF82}" name="ADM" dataDxfId="2" totalsRowDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{E184221B-D39C-481A-9EF0-7BBC0BDCFFB3}" name="ADM SUPLENTE" dataDxfId="1" totalsRowDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{7C167C76-67AF-4A26-8B9A-BCE2A4995E2A}" name="GESTOR(A)_x000a_ATUANTE" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{884CD221-7FDF-449F-BDDC-36A59A961922}" name="GESTOR SUPLENTE" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{4BAEAB60-D8F3-4A1C-A2A7-1AF80D70ECFB}" name="FISCAL NOMEADO" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{92B91F80-B146-424A-9B8F-B3A204D6D240}" name="MUNICIPIO" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{536E627B-103D-43E3-ADF4-5534C1B8AC84}" name="EMPRESA" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{6244ECFF-D04A-4C9E-9BB6-3E00642A9BA0}" name="%EXEC" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{E519A9AE-567A-406C-B69A-B1B53C257A70}" name="STATUS" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{682B89AE-0AB9-4B7F-8C3B-66D341320532}" name="FISCAL SUPLENTE" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{B76C21C5-382B-4784-B00B-25BF832EBF82}" name="ADM" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{E184221B-D39C-481A-9EF0-7BBC0BDCFFB3}" name="ADM SUPLENTE" dataDxfId="11" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3521,8 +3518,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,19 +3543,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
       <c r="L1" s="32"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3581,10 +3578,10 @@
         <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>132</v>
@@ -3598,7 +3595,7 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="38" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -3620,7 +3617,7 @@
         <v>0.25580000000000003</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>151</v>
@@ -3633,7 +3630,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3649,13 +3646,13 @@
         <v>27</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G4" s="27">
         <v>0</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>151</v>
@@ -3668,7 +3665,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -3690,7 +3687,7 @@
         <v>0.99670000000000003</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>145</v>
@@ -3703,7 +3700,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3725,7 +3722,7 @@
         <v>0.97860000000000003</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>151</v>
@@ -3740,7 +3737,7 @@
       <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -3762,7 +3759,7 @@
         <v>1.6500000000000001E-2</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>145</v>
@@ -3777,7 +3774,7 @@
       <c r="N7" s="31"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -3799,7 +3796,7 @@
         <v>0.38669999999999999</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>151</v>
@@ -3814,7 +3811,7 @@
       <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="38" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -3836,7 +3833,7 @@
         <v>0.9899</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>151</v>
@@ -3849,7 +3846,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -3871,7 +3868,7 @@
         <v>3.7699999999999997E-2</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>151</v>
@@ -3884,7 +3881,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -3906,7 +3903,7 @@
         <v>0.88560000000000005</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>145</v>
@@ -3919,7 +3916,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3941,7 +3938,7 @@
         <v>0.53190000000000004</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>151</v>
@@ -3954,7 +3951,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -3976,7 +3973,7 @@
         <v>0.1074</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>151</v>
@@ -3989,7 +3986,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="39" t="s">
         <v>110</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -4011,7 +4008,7 @@
         <v>0.54500000000000004</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>145</v>
@@ -4024,7 +4021,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="38" t="s">
         <v>96</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4046,7 +4043,7 @@
         <v>0.64100000000000001</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>145</v>
@@ -4059,7 +4056,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="39" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -4081,7 +4078,7 @@
         <v>0.71809999999999996</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>151</v>
@@ -4094,7 +4091,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="38" t="s">
         <v>98</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4116,7 +4113,7 @@
         <v>0.62</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>151</v>
@@ -4129,7 +4126,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="39" t="s">
         <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -4151,7 +4148,7 @@
         <v>0.2321</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>151</v>
@@ -4164,7 +4161,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -4186,7 +4183,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>148</v>
@@ -4199,7 +4196,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -4221,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>151</v>
@@ -4234,7 +4231,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -4256,7 +4253,7 @@
         <v>0.78049999999999997</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>148</v>
@@ -4269,7 +4266,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="39" t="s">
         <v>121</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -4291,7 +4288,7 @@
         <v>0.5</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>151</v>
@@ -4304,7 +4301,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="38" t="s">
         <v>118</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -4326,7 +4323,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>145</v>
@@ -4339,7 +4336,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -4361,7 +4358,7 @@
         <v>0.7903</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>148</v>
@@ -4374,7 +4371,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="38" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -4396,7 +4393,7 @@
         <v>0.78090000000000004</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>145</v>
@@ -4409,7 +4406,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -4431,7 +4428,7 @@
         <v>0.66039999999999999</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>148</v>
@@ -4444,7 +4441,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -4466,7 +4463,7 @@
         <v>0.86519999999999997</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>148</v>
@@ -4479,7 +4476,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -4501,7 +4498,7 @@
         <v>0.69730000000000003</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>148</v>
@@ -4575,19 +4572,19 @@
       <c r="M32"/>
     </row>
     <row r="33" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
       <c r="L33" s="33"/>
       <c r="M33"/>
     </row>
@@ -4611,10 +4608,10 @@
         <v>24</v>
       </c>
       <c r="G34" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H34" s="18" t="s">
         <v>161</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>162</v>
       </c>
       <c r="I34" s="18" t="s">
         <v>132</v>
@@ -4628,7 +4625,7 @@
       <c r="L34"/>
     </row>
     <row r="35" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="38" t="s">
         <v>112</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -4650,7 +4647,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>145</v>
@@ -4663,7 +4660,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="39" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -4685,7 +4682,7 @@
         <v>0.5746</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>145</v>
@@ -4698,7 +4695,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -4720,7 +4717,7 @@
         <v>0.84570000000000001</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>145</v>
@@ -4733,7 +4730,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="39" t="s">
         <v>76</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -4755,7 +4752,7 @@
         <v>0.99929999999999997</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>145</v>
@@ -4768,7 +4765,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="38" t="s">
         <v>77</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -4790,7 +4787,7 @@
         <v>0.79930000000000001</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>145</v>
@@ -4803,7 +4800,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="39" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -4825,7 +4822,7 @@
         <v>0.30669999999999997</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>145</v>
@@ -4838,7 +4835,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="38" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -4860,7 +4857,7 @@
         <v>0.96009999999999995</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>145</v>
@@ -4873,7 +4870,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="39" t="s">
         <v>115</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -4895,7 +4892,7 @@
         <v>1.5408999999999999</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I42" s="6" t="s">
         <v>145</v>
@@ -4908,7 +4905,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="38" t="s">
         <v>80</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -4930,7 +4927,7 @@
         <v>0.78459999999999996</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>145</v>
@@ -4943,7 +4940,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="39" t="s">
         <v>113</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -4965,7 +4962,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>145</v>
@@ -4978,7 +4975,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="38" t="s">
         <v>81</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -5000,7 +4997,7 @@
         <v>0.89959999999999996</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>145</v>
@@ -5011,13 +5008,13 @@
       <c r="K45" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="M45" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="N45" s="40"/>
+      <c r="M45" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="N45" s="46"/>
     </row>
     <row r="46" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="39" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="6" t="s">
@@ -5039,7 +5036,7 @@
         <v>0.97130000000000005</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>145</v>
@@ -5062,7 +5059,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="38" t="s">
         <v>130</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -5084,7 +5081,7 @@
         <v>0.80789999999999995</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>145</v>
@@ -5107,7 +5104,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="39" t="s">
         <v>83</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -5129,7 +5126,7 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>145</v>
@@ -5152,7 +5149,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="44" t="s">
+      <c r="A49" s="38" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -5174,7 +5171,7 @@
         <v>0.14130000000000001</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>145</v>
@@ -5253,24 +5250,24 @@
       <c r="M53" s="30"/>
     </row>
     <row r="54" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="41" t="s">
+      <c r="A54" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="43"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="49"/>
       <c r="L54" s="32"/>
-      <c r="M54" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="N54" s="39"/>
+      <c r="M54" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="N54" s="45"/>
       <c r="O54" s="35"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -5293,10 +5290,10 @@
         <v>24</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="I55" s="18" t="s">
         <v>132</v>
@@ -5309,7 +5306,7 @@
       </c>
       <c r="L55"/>
       <c r="M55" s="36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N55" s="37" cm="1">
         <f t="array" ref="N55">SUMPRODUCT(IF(ISERROR(FIND(M55, $D$3:$D$69)), 0, 1))</f>
@@ -5318,7 +5315,7 @@
       <c r="O55" s="31"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="40" t="s">
         <v>49</v>
       </c>
       <c r="B56" s="20" t="s">
@@ -5340,7 +5337,7 @@
         <v>0.6603</v>
       </c>
       <c r="H56" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>153</v>
@@ -5362,7 +5359,7 @@
       <c r="O56" s="31"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="41" t="s">
         <v>50</v>
       </c>
       <c r="B57" s="20" t="s">
@@ -5384,7 +5381,7 @@
         <v>0.51629999999999998</v>
       </c>
       <c r="H57" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I57" s="6" t="s">
         <v>153</v>
@@ -5401,12 +5398,12 @@
       </c>
       <c r="N57" s="37" cm="1">
         <f t="array" ref="N57">SUMPRODUCT(IF(ISERROR(FIND(M57, $D$3:$D$69)), 0, 1))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O57" s="31"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
+      <c r="A58" s="40" t="s">
         <v>126</v>
       </c>
       <c r="B58" s="20" t="s">
@@ -5428,7 +5425,7 @@
         <v>0.99219999999999997</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>153</v>
@@ -5450,7 +5447,7 @@
       <c r="O58" s="31"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="41" t="s">
         <v>128</v>
       </c>
       <c r="B59" s="20" t="s">
@@ -5472,7 +5469,7 @@
         <v>0.99539999999999995</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I59" s="6" t="s">
         <v>153</v>
@@ -5485,7 +5482,7 @@
       </c>
       <c r="L59"/>
       <c r="M59" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N59" s="37" cm="1">
         <f t="array" ref="N59">SUMPRODUCT(IF(ISERROR(FIND(M59, $D$3:$D$69)), 0, 1))</f>
@@ -5494,7 +5491,7 @@
       <c r="O59" s="31"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
+      <c r="A60" s="40" t="s">
         <v>51</v>
       </c>
       <c r="B60" s="20" t="s">
@@ -5516,7 +5513,7 @@
         <v>0.43519999999999998</v>
       </c>
       <c r="H60" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I60" s="6" t="s">
         <v>153</v>
@@ -5533,12 +5530,12 @@
       </c>
       <c r="N60" s="37" cm="1">
         <f t="array" ref="N60">SUMPRODUCT(IF(ISERROR(FIND(M60, $D$3:$D$69)), 0, 1))</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O60" s="31"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="47" t="s">
+      <c r="A61" s="41" t="s">
         <v>52</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -5560,7 +5557,7 @@
         <v>0.5958</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I61" s="6" t="s">
         <v>153</v>
@@ -5582,7 +5579,7 @@
       <c r="O61" s="31"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="46" t="s">
+      <c r="A62" s="40" t="s">
         <v>53</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -5604,7 +5601,7 @@
         <v>0.84209999999999996</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I62" s="6" t="s">
         <v>153</v>
@@ -5617,7 +5614,7 @@
       </c>
       <c r="L62"/>
       <c r="M62" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N62" s="37" cm="1">
         <f t="array" ref="N62">SUMPRODUCT(IF(ISERROR(FIND(M62, $D$3:$D$69)), 0, 1))</f>
@@ -5626,7 +5623,7 @@
       <c r="O62" s="31"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="48" t="s">
+      <c r="A63" s="42" t="s">
         <v>100</v>
       </c>
       <c r="B63" s="16" t="s">
@@ -5648,7 +5645,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I63" s="15" t="s">
         <v>157</v>
@@ -5671,7 +5668,7 @@
       <c r="O63" s="31"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
+      <c r="A64" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B64" s="16" t="s">
@@ -5693,7 +5690,7 @@
         <v>0.85919999999999996</v>
       </c>
       <c r="H64" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>157</v>
@@ -5711,7 +5708,7 @@
       <c r="O64" s="31"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="43" t="s">
         <v>107</v>
       </c>
       <c r="B65" s="16" t="s">
@@ -5734,7 +5731,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H65" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I65" s="15" t="s">
         <v>157</v>
@@ -5752,7 +5749,7 @@
       <c r="O65" s="31"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="46" t="s">
+      <c r="A66" s="40" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -5774,7 +5771,7 @@
         <v>0.87860000000000005</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I66" s="21" t="s">
         <v>157</v>
@@ -5791,7 +5788,7 @@
       <c r="O66" s="31"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="47" t="s">
+      <c r="A67" s="41" t="s">
         <v>123</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -5801,7 +5798,7 @@
         <v>140</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>124</v>
@@ -5813,7 +5810,7 @@
         <v>0</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I67" s="21" t="s">
         <v>157</v>
@@ -5828,7 +5825,7 @@
       <c r="M67"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="46" t="s">
+      <c r="A68" s="40" t="s">
         <v>55</v>
       </c>
       <c r="B68" s="5" t="s">
@@ -5850,7 +5847,7 @@
         <v>0.97019999999999995</v>
       </c>
       <c r="H68" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I68" s="21" t="s">
         <v>157</v>
@@ -5865,7 +5862,7 @@
       <c r="M68"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="47" t="s">
+      <c r="A69" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -5887,7 +5884,7 @@
         <v>0.31530000000000002</v>
       </c>
       <c r="H69" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I69" s="21" t="s">
         <v>157</v>
@@ -6066,7 +6063,7 @@
   </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="K56:K69" calculatedColumn="1"/>
-    <ignoredError sqref="N55:N63" emptyCellReference="1"/>
+    <ignoredError sqref="N55:N56 N58:N63" emptyCellReference="1"/>
   </ignoredErrors>
   <tableParts count="3">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
feat: Implement user authentication and state management.
</commit_message>
<xml_diff>
--- a/CONTROLES POR COMISSÃO E GESTORES.xlsx
+++ b/CONTROLES POR COMISSÃO E GESTORES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDICOES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0340A459-02F2-4CB2-8DAF-A2D293433B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29004E44-23AB-4C5C-B281-F2FD893FD0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="454" xr2:uid="{B96EB9A8-6169-46F2-89FD-740783B0C7B5}"/>
   </bookViews>
@@ -3519,7 +3519,7 @@
   <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="M75" sqref="M75"/>
+      <selection activeCell="A64" sqref="A64:K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,7 +5100,7 @@
 ATUANTE],M47)+COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],M47)+COUNTIF(Tabela3[GESTOR(A)
 ATUANTE],M47)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
@@ -5217,7 +5217,7 @@
 ATUANTE],M50)+COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],M50)+COUNTIF(Tabela3[GESTOR(A)
 ATUANTE],M50)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
@@ -5671,11 +5671,11 @@
       <c r="A64" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="16" t="s">
         <v>141</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>140</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>159</v>
@@ -5935,7 +5935,7 @@
       <c r="C72" s="13">
         <f>COUNTIF(Tabela2[GESTOR(A)
 ATUANTE],B72)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N72" s="31"/>
     </row>
@@ -6063,7 +6063,7 @@
   </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="K56:K69" calculatedColumn="1"/>
-    <ignoredError sqref="N55:N56 N58:N63" emptyCellReference="1"/>
+    <ignoredError sqref="N55:N63" emptyCellReference="1"/>
   </ignoredErrors>
   <tableParts count="3">
     <tablePart r:id="rId2"/>

</xml_diff>